<commit_message>
gebiet_id einfügen in create_dataset
</commit_message>
<xml_diff>
--- a/5204_energie_test.xlsx
+++ b/5204_energie_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E98E633-4567-4C0F-9E77-2DD9CD7215B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C0B08A-175B-45A9-8C58-32D4FF9658EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
     <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -485,22 +485,22 @@
     <t>px</t>
   </si>
   <si>
+    <t>Bevölkerungstyp</t>
+  </si>
+  <si>
+    <t>Ständige und nichtständige Wohnbevölkerung</t>
+  </si>
+  <si>
+    <t>Personen</t>
+  </si>
+  <si>
+    <t>Statistik der Bevölkerung und der Haushalte STATPOP (BFS)</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>8100,ZH</t>
-  </si>
-  <si>
-    <t>Bevölkerungstyp</t>
-  </si>
-  <si>
-    <t>Ständige und nichtständige Wohnbevölkerung</t>
-  </si>
-  <si>
-    <t>Personen</t>
-  </si>
-  <si>
-    <t>Statistik der Bevölkerung und der Haushalte STATPOP (BFS)</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
 </sst>
 </file>
@@ -4088,7 +4088,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4376,13 +4376,13 @@
         <v>97</v>
       </c>
       <c r="M4" s="25" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="N4" s="25" t="s">
         <v>89</v>
       </c>
       <c r="O4" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P4" s="25">
         <v>1</v>
@@ -4394,19 +4394,19 @@
       <c r="S4" s="25"/>
       <c r="T4" s="25"/>
       <c r="U4" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="V4" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="V4" s="25" t="s">
+      <c r="X4" s="25" t="s">
         <v>117</v>
-      </c>
-      <c r="X4" s="25" t="s">
-        <v>118</v>
       </c>
       <c r="Y4" s="25" t="s">
         <v>91</v>
       </c>
       <c r="AA4" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -5249,26 +5249,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D6EF8296678614C82595E073A935E63" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2c357ece3d19c143a9e4a1e033fa04b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c16c412-41a7-483e-8458-9b4c6e041c8c" xmlns:ns3="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78066d3103febb3f607343910020d0d2" ns2:_="" ns3:_="">
     <xsd:import namespace="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
@@ -5473,10 +5453,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
+    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5499,20 +5510,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
-    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>